<commit_message>
delete temp excel file
</commit_message>
<xml_diff>
--- a/schema.xlsx
+++ b/schema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="-440" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -219,8 +219,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -255,7 +262,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="36">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -284,6 +291,13 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -613,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="R19" activeCellId="1" sqref="R13:R15 R19:R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -726,8 +740,8 @@
         <v>16</v>
       </c>
       <c r="J10" t="str">
-        <f>I10</f>
-        <v>music</v>
+        <f t="shared" ref="J10:J12" si="0">"("&amp;H10&amp;","&amp;I10&amp;")"</f>
+        <v>(1,music)</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -781,7 +795,7 @@
         <v>20131206</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" ref="G11:G19" si="0">"("&amp;B11&amp;","&amp;C11&amp;","&amp;D11&amp;","&amp;E11&amp;","&amp;F11&amp;")"</f>
+        <f t="shared" ref="G11:G19" si="1">"("&amp;B11&amp;","&amp;C11&amp;","&amp;D11&amp;","&amp;E11&amp;","&amp;F11&amp;")"</f>
         <v>(hurricane sandy victims,3,20000,20131004,20131206)</v>
       </c>
       <c r="H11">
@@ -791,8 +805,8 @@
         <v>17</v>
       </c>
       <c r="J11" t="str">
-        <f>I11</f>
-        <v>books</v>
+        <f t="shared" si="0"/>
+        <v>(2,books)</v>
       </c>
       <c r="K11">
         <f>K10+1</f>
@@ -806,7 +820,7 @@
         <v>21</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" ref="N11:N29" si="1">"("&amp;L11&amp;","&amp;M11&amp;")"</f>
+        <f t="shared" ref="N11:N29" si="2">"("&amp;L11&amp;","&amp;M11&amp;")"</f>
         <v>(Amanda,21)</v>
       </c>
       <c r="O11">
@@ -814,7 +828,6 @@
         <v>2</v>
       </c>
       <c r="P11">
-        <f>P10+1000</f>
         <v>2000</v>
       </c>
       <c r="Q11">
@@ -826,7 +839,7 @@
         <v>2</v>
       </c>
       <c r="S11" t="str">
-        <f t="shared" ref="S11:S39" si="2">"("&amp;P11&amp;","&amp;Q11&amp;","&amp;R11&amp;")"</f>
+        <f t="shared" ref="S11:S39" si="3">"("&amp;P11&amp;","&amp;Q11&amp;","&amp;R11&amp;")"</f>
         <v>(2000,2,2)</v>
       </c>
     </row>
@@ -844,15 +857,15 @@
         <v>15000</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12:E19" si="3">E11+1</f>
+        <f t="shared" ref="E12:E19" si="4">E11+1</f>
         <v>20131005</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:F19" si="4">F11+3</f>
+        <f t="shared" ref="F12:F19" si="5">F11+3</f>
         <v>20131209</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(women in programming,3,15000,20131005,20131209)</v>
       </c>
       <c r="H12">
@@ -862,30 +875,29 @@
         <v>18</v>
       </c>
       <c r="J12" t="str">
-        <f>I12</f>
-        <v>charity</v>
+        <f t="shared" si="0"/>
+        <v>(3,charity)</v>
       </c>
       <c r="K12">
-        <f t="shared" ref="K12:K29" si="5">K11+1</f>
+        <f t="shared" ref="K12:K29" si="6">K11+1</f>
         <v>3</v>
       </c>
       <c r="L12" t="s">
         <v>31</v>
       </c>
       <c r="M12">
-        <f t="shared" ref="M12:M29" si="6">M11+1</f>
+        <f t="shared" ref="M12:M29" si="7">M11+1</f>
         <v>22</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Anders,22)</v>
       </c>
       <c r="O12">
-        <f t="shared" ref="O12:O39" si="7">O11+1</f>
+        <f t="shared" ref="O12:O39" si="8">O11+1</f>
         <v>3</v>
       </c>
       <c r="P12">
-        <f t="shared" ref="P12:P39" si="8">P11+1000</f>
         <v>3000</v>
       </c>
       <c r="Q12">
@@ -897,7 +909,7 @@
         <v>3</v>
       </c>
       <c r="S12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(3000,3,3)</v>
       </c>
     </row>
@@ -915,38 +927,37 @@
         <v>30000</v>
       </c>
       <c r="E13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20131006</v>
       </c>
       <c r="F13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20131212</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(pop up philharmonic,1,30000,20131006,20131212)</v>
       </c>
       <c r="K13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="L13" t="s">
         <v>32</v>
       </c>
       <c r="M13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>23</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Bana,23)</v>
       </c>
       <c r="O13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="P13">
-        <f t="shared" si="8"/>
         <v>4000</v>
       </c>
       <c r="Q13">
@@ -958,7 +969,7 @@
         <v>4</v>
       </c>
       <c r="S13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(4000,4,4)</v>
       </c>
     </row>
@@ -976,38 +987,37 @@
         <v>50000</v>
       </c>
       <c r="E14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20131007</v>
       </c>
       <c r="F14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20131215</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(kindergarten muscians,1,50000,20131007,20131215)</v>
       </c>
       <c r="K14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="L14" t="s">
         <v>33</v>
       </c>
       <c r="M14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Brendan,24)</v>
       </c>
       <c r="O14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="P14">
-        <f t="shared" si="8"/>
         <v>5000</v>
       </c>
       <c r="Q14">
@@ -1019,7 +1029,7 @@
         <v>5</v>
       </c>
       <c r="S14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(5000,5,5)</v>
       </c>
     </row>
@@ -1037,38 +1047,37 @@
         <v>25000</v>
       </c>
       <c r="E15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20131008</v>
       </c>
       <c r="F15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20131218</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(flash dance in central park,1,25000,20131008,20131218)</v>
       </c>
       <c r="K15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="L15" t="s">
         <v>34</v>
       </c>
       <c r="M15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Charlotte,25)</v>
       </c>
       <c r="O15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="P15">
-        <f t="shared" si="8"/>
         <v>6000</v>
       </c>
       <c r="Q15">
@@ -1080,7 +1089,7 @@
         <v>6</v>
       </c>
       <c r="S15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(6000,6,6)</v>
       </c>
     </row>
@@ -1098,38 +1107,37 @@
         <v>7000</v>
       </c>
       <c r="E16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20131009</v>
       </c>
       <c r="F16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20131221</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(my autobiography,2,7000,20131009,20131221)</v>
       </c>
       <c r="K16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="L16" t="s">
         <v>35</v>
       </c>
       <c r="M16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
       <c r="N16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Chris,26)</v>
       </c>
       <c r="O16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="P16">
-        <f t="shared" si="8"/>
         <v>7000</v>
       </c>
       <c r="Q16">
@@ -1141,7 +1149,7 @@
         <v>7</v>
       </c>
       <c r="S16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(7000,7,7)</v>
       </c>
     </row>
@@ -1159,38 +1167,37 @@
         <v>36000</v>
       </c>
       <c r="E17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20131010</v>
       </c>
       <c r="F17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20131224</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(memoirs of a programmer,2,36000,20131010,20131224)</v>
       </c>
       <c r="K17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="L17" t="s">
         <v>36</v>
       </c>
       <c r="M17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
       <c r="N17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Dave,27)</v>
       </c>
       <c r="O17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="P17">
-        <f t="shared" si="8"/>
         <v>8000</v>
       </c>
       <c r="Q17">
@@ -1202,7 +1209,7 @@
         <v>8</v>
       </c>
       <c r="S17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(8000,8,8)</v>
       </c>
     </row>
@@ -1220,38 +1227,37 @@
         <v>48000</v>
       </c>
       <c r="E18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20131011</v>
       </c>
       <c r="F18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20131227</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(how to count again,2,48000,20131011,20131227)</v>
       </c>
       <c r="K18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="L18" t="s">
         <v>37</v>
       </c>
       <c r="M18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="N18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Edina,28)</v>
       </c>
       <c r="O18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="P18">
-        <f t="shared" si="8"/>
         <v>9000</v>
       </c>
       <c r="Q18">
@@ -1263,7 +1269,7 @@
         <v>9</v>
       </c>
       <c r="S18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(9000,9,9)</v>
       </c>
     </row>
@@ -1281,38 +1287,37 @@
         <v>100000</v>
       </c>
       <c r="E19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20131012</v>
       </c>
       <c r="F19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20131230</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(teach the world to read music,1,100000,20131012,20131230)</v>
       </c>
       <c r="K19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="L19" t="s">
         <v>38</v>
       </c>
       <c r="M19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>29</v>
       </c>
       <c r="N19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Emily,29)</v>
       </c>
       <c r="O19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="P19">
-        <f t="shared" si="8"/>
         <v>10000</v>
       </c>
       <c r="Q19">
@@ -1324,32 +1329,31 @@
         <v>10</v>
       </c>
       <c r="S19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(10000,10,10)</v>
       </c>
     </row>
     <row r="20" spans="1:19">
       <c r="K20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="L20" t="s">
         <v>39</v>
       </c>
       <c r="M20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="N20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Greg,30)</v>
       </c>
       <c r="O20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="P20">
-        <f t="shared" si="8"/>
         <v>11000</v>
       </c>
       <c r="Q20">
@@ -1360,32 +1364,31 @@
         <v>1</v>
       </c>
       <c r="S20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(11000,11,1)</v>
       </c>
     </row>
     <row r="21" spans="1:19">
       <c r="K21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="L21" t="s">
         <v>40</v>
       </c>
       <c r="M21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>31</v>
       </c>
       <c r="N21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Ian,31)</v>
       </c>
       <c r="O21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="P21">
-        <f t="shared" si="8"/>
         <v>12000</v>
       </c>
       <c r="Q21">
@@ -1397,32 +1400,31 @@
         <v>2</v>
       </c>
       <c r="S21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(12000,12,2)</v>
       </c>
     </row>
     <row r="22" spans="1:19">
       <c r="K22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="L22" t="s">
         <v>41</v>
       </c>
       <c r="M22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>32</v>
       </c>
       <c r="N22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Iris,32)</v>
       </c>
       <c r="O22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="P22">
-        <f t="shared" si="8"/>
         <v>13000</v>
       </c>
       <c r="Q22">
@@ -1434,32 +1436,31 @@
         <v>3</v>
       </c>
       <c r="S22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(13000,13,3)</v>
       </c>
     </row>
     <row r="23" spans="1:19">
       <c r="K23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="L23" t="s">
         <v>42</v>
       </c>
       <c r="M23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
       <c r="N23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Ivan,33)</v>
       </c>
       <c r="O23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="P23">
-        <f t="shared" si="8"/>
         <v>14000</v>
       </c>
       <c r="Q23">
@@ -1471,32 +1472,31 @@
         <v>4</v>
       </c>
       <c r="S23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(14000,14,4)</v>
       </c>
     </row>
     <row r="24" spans="1:19">
       <c r="K24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="L24" t="s">
         <v>43</v>
       </c>
       <c r="M24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>34</v>
       </c>
       <c r="N24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(James,34)</v>
       </c>
       <c r="O24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="P24">
-        <f t="shared" si="8"/>
         <v>15000</v>
       </c>
       <c r="Q24">
@@ -1508,32 +1508,31 @@
         <v>5</v>
       </c>
       <c r="S24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(15000,15,5)</v>
       </c>
     </row>
     <row r="25" spans="1:19">
       <c r="K25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="L25" t="s">
         <v>44</v>
       </c>
       <c r="M25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
       <c r="N25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Jeanne,35)</v>
       </c>
       <c r="O25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="P25">
-        <f t="shared" si="8"/>
         <v>16000</v>
       </c>
       <c r="Q25">
@@ -1545,32 +1544,31 @@
         <v>6</v>
       </c>
       <c r="S25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(16000,16,6)</v>
       </c>
     </row>
     <row r="26" spans="1:19">
       <c r="K26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="L26" t="s">
         <v>45</v>
       </c>
       <c r="M26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="N26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Joe,36)</v>
       </c>
       <c r="O26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="P26">
-        <f t="shared" si="8"/>
         <v>17000</v>
       </c>
       <c r="Q26">
@@ -1582,32 +1580,31 @@
         <v>7</v>
       </c>
       <c r="S26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(17000,17,7)</v>
       </c>
     </row>
     <row r="27" spans="1:19">
       <c r="K27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="L27" t="s">
         <v>46</v>
       </c>
       <c r="M27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>37</v>
       </c>
       <c r="N27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(John,37)</v>
       </c>
       <c r="O27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="P27">
-        <f t="shared" si="8"/>
         <v>18000</v>
       </c>
       <c r="Q27">
@@ -1619,32 +1616,31 @@
         <v>8</v>
       </c>
       <c r="S27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(18000,18,8)</v>
       </c>
     </row>
     <row r="28" spans="1:19">
       <c r="K28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="L28" t="s">
         <v>47</v>
       </c>
       <c r="M28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>38</v>
       </c>
       <c r="N28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Josh,38)</v>
       </c>
       <c r="O28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="P28">
-        <f t="shared" si="8"/>
         <v>19000</v>
       </c>
       <c r="Q28">
@@ -1656,32 +1652,31 @@
         <v>9</v>
       </c>
       <c r="S28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(19000,19,9)</v>
       </c>
     </row>
     <row r="29" spans="1:19">
       <c r="K29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="L29" t="s">
         <v>48</v>
       </c>
       <c r="M29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39</v>
       </c>
       <c r="N29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Kyle,39)</v>
       </c>
       <c r="O29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="P29">
-        <f t="shared" si="8"/>
         <v>20000</v>
       </c>
       <c r="Q29">
@@ -1693,17 +1688,16 @@
         <v>10</v>
       </c>
       <c r="S29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(20000,20,10)</v>
       </c>
     </row>
     <row r="30" spans="1:19">
       <c r="O30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="P30">
-        <f t="shared" si="8"/>
         <v>21000</v>
       </c>
       <c r="Q30">
@@ -1713,17 +1707,16 @@
         <v>1</v>
       </c>
       <c r="S30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(21000,1,1)</v>
       </c>
     </row>
     <row r="31" spans="1:19">
       <c r="O31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="P31">
-        <f t="shared" si="8"/>
         <v>22000</v>
       </c>
       <c r="Q31">
@@ -1734,17 +1727,16 @@
         <v>2</v>
       </c>
       <c r="S31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(22000,2,2)</v>
       </c>
     </row>
     <row r="32" spans="1:19">
       <c r="O32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="P32">
-        <f t="shared" si="8"/>
         <v>23000</v>
       </c>
       <c r="Q32">
@@ -1755,17 +1747,16 @@
         <v>3</v>
       </c>
       <c r="S32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(23000,3,3)</v>
       </c>
     </row>
     <row r="33" spans="15:19">
       <c r="O33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="P33">
-        <f t="shared" si="8"/>
         <v>24000</v>
       </c>
       <c r="Q33">
@@ -1776,17 +1767,16 @@
         <v>4</v>
       </c>
       <c r="S33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(24000,4,4)</v>
       </c>
     </row>
     <row r="34" spans="15:19">
       <c r="O34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
       <c r="P34">
-        <f t="shared" si="8"/>
         <v>25000</v>
       </c>
       <c r="Q34">
@@ -1798,17 +1788,16 @@
         <v>5</v>
       </c>
       <c r="S34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(25000,5,5)</v>
       </c>
     </row>
     <row r="35" spans="15:19">
       <c r="O35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="P35">
-        <f t="shared" si="8"/>
         <v>26000</v>
       </c>
       <c r="Q35">
@@ -1820,17 +1809,16 @@
         <v>6</v>
       </c>
       <c r="S35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(26000,6,6)</v>
       </c>
     </row>
     <row r="36" spans="15:19">
       <c r="O36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
       <c r="P36">
-        <f t="shared" si="8"/>
         <v>27000</v>
       </c>
       <c r="Q36">
@@ -1842,17 +1830,16 @@
         <v>7</v>
       </c>
       <c r="S36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(27000,7,7)</v>
       </c>
     </row>
     <row r="37" spans="15:19">
       <c r="O37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28</v>
       </c>
       <c r="P37">
-        <f t="shared" si="8"/>
         <v>28000</v>
       </c>
       <c r="Q37">
@@ -1864,17 +1851,16 @@
         <v>8</v>
       </c>
       <c r="S37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(28000,8,8)</v>
       </c>
     </row>
     <row r="38" spans="15:19">
       <c r="O38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>29</v>
       </c>
       <c r="P38">
-        <f t="shared" si="8"/>
         <v>29000</v>
       </c>
       <c r="Q38">
@@ -1886,17 +1872,16 @@
         <v>9</v>
       </c>
       <c r="S38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(29000,9,9)</v>
       </c>
     </row>
     <row r="39" spans="15:19">
       <c r="O39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>30</v>
       </c>
       <c r="P39">
-        <f t="shared" si="8"/>
         <v>30000</v>
       </c>
       <c r="Q39">
@@ -1908,8 +1893,14 @@
         <v>10</v>
       </c>
       <c r="S39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(30000,10,10)</v>
+      </c>
+    </row>
+    <row r="40" spans="15:19">
+      <c r="P40">
+        <f>SUM(P10:P39)</f>
+        <v>465000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>